<commit_message>
read data from testng xml
</commit_message>
<xml_diff>
--- a/CCInfo.xlsx
+++ b/CCInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shiva/Documents/SDETIntenshipProgram/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E9F4D36-A1DE-BA41-A5E0-5EFD6738BCFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A4D3D3-54FE-8F4C-9F69-BBC7059E4845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" activeTab="1" xr2:uid="{FFEF8329-5C5A-4353-808D-92513DF928EE}"/>
   </bookViews>
@@ -869,7 +869,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>